<commit_message>
docs: update migration document to remove outdated columns and clarify dataset changes #1486
</commit_message>
<xml_diff>
--- a/support/specifications/flat-file/nyher-fhir-ig-example/Consolidated NYHER FHIR IG Examples.xlsx
+++ b/support/specifications/flat-file/nyher-fhir-ig-example/Consolidated NYHER FHIR IG Examples.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12300" activeTab="1"/>
+    <workbookView windowWidth="23040" windowHeight="9120" firstSheet="5" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="QE_ADMIN" sheetId="1" r:id="rId1"/>
@@ -1167,6 +1167,50 @@
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     resourceType ='Organization'-&gt;identifier-&gt;system</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AI1" authorId="4">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t>Megin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t xml:space="preserve">
+resourceType ='Consent'-&gt;meta-&gt;lastUpdated</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AJ1" authorId="4">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t>Megin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t xml:space="preserve">
+resourceType ='Encounter'-&gt;meta-&gt;lastUpdated</t>
         </r>
       </text>
     </comment>
@@ -1802,12 +1846,35 @@
         </r>
       </text>
     </comment>
+    <comment ref="AP1" authorId="6">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t>Megin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t xml:space="preserve">
+This time will be found in the FHIR Observation(SexualOrientation) resource -&gt;meta -&gt; lastUpdated
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1278" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1296" uniqueCount="363">
   <si>
     <t>PATIENT_MR_ID_VALUE</t>
   </si>
@@ -2466,6 +2533,12 @@
     <t>SCREENING_ENTITY_ID_CODE_SYSTEM</t>
   </si>
   <si>
+    <t>CONSENT_LAST_UPDATED</t>
+  </si>
+  <si>
+    <t>ENCOUNTER_LAST_UPDATED</t>
+  </si>
+  <si>
     <t>FLD</t>
   </si>
   <si>
@@ -2646,6 +2719,9 @@
     <t>PATIENT_LAST_UPDATED</t>
   </si>
   <si>
+    <t>SEXUAL_ORIENTATION_LAST_UPDATED</t>
+  </si>
+  <si>
     <t>AA12345C</t>
   </si>
   <si>
@@ -2805,18 +2881,12 @@
     <t>DATA_ABSENT_REASON_TEXT</t>
   </si>
   <si>
-    <t>CONSENT_LAST_UPDATED</t>
-  </si>
-  <si>
     <t>CONSENT_POLICY_AUTHORITY</t>
   </si>
   <si>
     <t>CONSENT_PROVISION_TYPE</t>
   </si>
   <si>
-    <t>ENCOUNTER_LAST_UPDATED</t>
-  </si>
-  <si>
     <t>PATIENT_MA_ID_VALUE</t>
   </si>
   <si>
@@ -2893,9 +2963,6 @@
   </si>
   <si>
     <t>SEXUAL_ORIENTATION_VALUE_CODE_SYSTEM_NAME</t>
-  </si>
-  <si>
-    <t>SEXUAL_ORIENTATION_LAST_UPDATED</t>
   </si>
 </sst>
 </file>
@@ -2909,7 +2976,7 @@
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="34">
+  <fonts count="35">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2991,6 +3058,12 @@
       <sz val="8.2"/>
       <color rgb="FF2A6496"/>
       <name val="Verdana"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <charset val="134"/>
     </font>
     <font>
@@ -3493,14 +3566,11 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -3509,119 +3579,122 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3693,7 +3766,8 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="178" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="6"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="22" applyFont="1" applyFill="1" applyAlignment="1" quotePrefix="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="23" applyFont="1" applyFill="1" applyAlignment="1" quotePrefix="1"/>
   </cellXfs>
@@ -4041,25 +4115,25 @@
       <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="22.1416666666667" customWidth="1"/>
-    <col min="2" max="2" width="11.2833333333333" customWidth="1"/>
-    <col min="3" max="3" width="14.8583333333333" customWidth="1"/>
-    <col min="4" max="4" width="25.8583333333333" customWidth="1"/>
-    <col min="5" max="5" width="28.1416666666667" customWidth="1"/>
-    <col min="6" max="6" width="36.5666666666667" customWidth="1"/>
-    <col min="7" max="7" width="28.1416666666667" customWidth="1"/>
-    <col min="8" max="8" width="18.5666666666667" customWidth="1"/>
-    <col min="9" max="9" width="34.8583333333333" customWidth="1"/>
-    <col min="10" max="10" width="13.1416666666667" customWidth="1"/>
-    <col min="11" max="11" width="14.7083333333333" customWidth="1"/>
+    <col min="1" max="1" width="22.1388888888889" customWidth="1"/>
+    <col min="2" max="2" width="11.287037037037" customWidth="1"/>
+    <col min="3" max="3" width="14.8611111111111" customWidth="1"/>
+    <col min="4" max="4" width="25.8611111111111" customWidth="1"/>
+    <col min="5" max="5" width="28.1388888888889" customWidth="1"/>
+    <col min="6" max="6" width="36.5648148148148" customWidth="1"/>
+    <col min="7" max="7" width="28.1388888888889" customWidth="1"/>
+    <col min="8" max="8" width="18.5648148148148" customWidth="1"/>
+    <col min="9" max="9" width="34.8611111111111" customWidth="1"/>
+    <col min="10" max="10" width="13.1388888888889" customWidth="1"/>
+    <col min="11" max="11" width="14.7037037037037" customWidth="1"/>
     <col min="12" max="12" width="12" customWidth="1"/>
     <col min="13" max="13" width="18" customWidth="1"/>
     <col min="14" max="14" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" spans="1:14">
+    <row r="1" spans="1:14">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -4103,7 +4177,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" ht="30" spans="1:14">
+    <row r="2" ht="28.8" spans="1:14">
       <c r="A2" s="8">
         <v>11223344</v>
       </c>
@@ -4159,36 +4233,36 @@
   <sheetPr/>
   <dimension ref="A1:V31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="S4" sqref="S4"/>
+    <sheetView topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="22.1416666666667" customWidth="1"/>
-    <col min="2" max="2" width="11.2833333333333" customWidth="1"/>
-    <col min="3" max="3" width="14.8583333333333" customWidth="1"/>
-    <col min="4" max="4" width="17.2833333333333" customWidth="1"/>
-    <col min="5" max="6" width="26.8583333333333" customWidth="1"/>
-    <col min="7" max="7" width="16.8583333333333" customWidth="1"/>
-    <col min="8" max="8" width="36.5666666666667" customWidth="1"/>
-    <col min="9" max="9" width="31.425" customWidth="1"/>
-    <col min="10" max="10" width="16.1416666666667" customWidth="1"/>
-    <col min="11" max="11" width="36.5666666666667" customWidth="1"/>
-    <col min="12" max="12" width="30.7083333333333" customWidth="1"/>
-    <col min="13" max="13" width="14.5666666666667" customWidth="1"/>
-    <col min="14" max="14" width="27.2833333333333" customWidth="1"/>
-    <col min="15" max="15" width="29.1416666666667" customWidth="1"/>
-    <col min="16" max="16" width="36.1416666666667" customWidth="1"/>
-    <col min="17" max="17" width="35.425" customWidth="1"/>
-    <col min="18" max="18" width="27.8583333333333" customWidth="1"/>
-    <col min="19" max="19" width="30.1416666666667" customWidth="1"/>
-    <col min="20" max="20" width="27.1416666666667" customWidth="1"/>
-    <col min="21" max="21" width="30.1416666666667" customWidth="1"/>
-    <col min="22" max="22" width="25.8583333333333" customWidth="1"/>
+    <col min="1" max="1" width="22.1388888888889" customWidth="1"/>
+    <col min="2" max="2" width="11.287037037037" customWidth="1"/>
+    <col min="3" max="3" width="14.8611111111111" customWidth="1"/>
+    <col min="4" max="4" width="17.287037037037" customWidth="1"/>
+    <col min="5" max="6" width="26.8611111111111" customWidth="1"/>
+    <col min="7" max="7" width="16.8611111111111" customWidth="1"/>
+    <col min="8" max="8" width="36.5648148148148" customWidth="1"/>
+    <col min="9" max="9" width="31.4259259259259" customWidth="1"/>
+    <col min="10" max="10" width="16.1388888888889" customWidth="1"/>
+    <col min="11" max="11" width="36.5648148148148" customWidth="1"/>
+    <col min="12" max="12" width="30.712962962963" customWidth="1"/>
+    <col min="13" max="13" width="14.5648148148148" customWidth="1"/>
+    <col min="14" max="14" width="27.287037037037" customWidth="1"/>
+    <col min="15" max="15" width="29.1388888888889" customWidth="1"/>
+    <col min="16" max="16" width="36.1388888888889" customWidth="1"/>
+    <col min="17" max="17" width="35.4259259259259" customWidth="1"/>
+    <col min="18" max="18" width="27.8611111111111" customWidth="1"/>
+    <col min="19" max="19" width="30.1388888888889" customWidth="1"/>
+    <col min="20" max="20" width="27.1388888888889" customWidth="1"/>
+    <col min="21" max="21" width="30.1388888888889" customWidth="1"/>
+    <col min="22" max="22" width="25.8611111111111" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" spans="1:22">
+    <row r="1" spans="1:22">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -4256,7 +4330,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" ht="45" spans="1:22">
+    <row r="2" ht="43.2" spans="1:22">
       <c r="A2" s="8">
         <v>11223344</v>
       </c>
@@ -4269,7 +4343,7 @@
       <c r="D2" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E2" s="33" t="s">
+      <c r="E2" s="34" t="s">
         <v>46</v>
       </c>
       <c r="F2" s="8" t="s">
@@ -4320,7 +4394,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" ht="45" spans="1:22">
+    <row r="3" ht="43.2" spans="1:22">
       <c r="A3" s="8">
         <v>11223344</v>
       </c>
@@ -4333,7 +4407,7 @@
       <c r="D3" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="33" t="s">
+      <c r="E3" s="34" t="s">
         <v>46</v>
       </c>
       <c r="F3" s="8" t="s">
@@ -4384,7 +4458,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" ht="45" spans="1:22">
+    <row r="4" ht="43.2" spans="1:22">
       <c r="A4" s="8">
         <v>11223344</v>
       </c>
@@ -4397,7 +4471,7 @@
       <c r="D4" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="33" t="s">
+      <c r="E4" s="34" t="s">
         <v>46</v>
       </c>
       <c r="F4" s="8" t="s">
@@ -4448,7 +4522,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" ht="45" spans="1:22">
+    <row r="5" ht="43.2" spans="1:22">
       <c r="A5" s="8">
         <v>11223344</v>
       </c>
@@ -4461,7 +4535,7 @@
       <c r="D5" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E5" s="33" t="s">
+      <c r="E5" s="34" t="s">
         <v>46</v>
       </c>
       <c r="F5" s="8" t="s">
@@ -4512,7 +4586,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" ht="60" spans="1:22">
+    <row r="6" ht="57.6" spans="1:22">
       <c r="A6" s="8">
         <v>11223344</v>
       </c>
@@ -4525,7 +4599,7 @@
       <c r="D6" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E6" s="33" t="s">
+      <c r="E6" s="34" t="s">
         <v>46</v>
       </c>
       <c r="F6" s="8" t="s">
@@ -4576,7 +4650,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" ht="45" spans="1:22">
+    <row r="7" ht="43.2" spans="1:22">
       <c r="A7" s="8">
         <v>11223344</v>
       </c>
@@ -4589,7 +4663,7 @@
       <c r="D7" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="33" t="s">
+      <c r="E7" s="34" t="s">
         <v>46</v>
       </c>
       <c r="F7" s="8" t="s">
@@ -4640,7 +4714,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" ht="45" spans="1:22">
+    <row r="8" ht="43.2" spans="1:22">
       <c r="A8" s="8">
         <v>11223344</v>
       </c>
@@ -4653,7 +4727,7 @@
       <c r="D8" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="33" t="s">
+      <c r="E8" s="34" t="s">
         <v>46</v>
       </c>
       <c r="F8" s="8" t="s">
@@ -4704,7 +4778,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" ht="45" spans="1:22">
+    <row r="9" ht="43.2" spans="1:22">
       <c r="A9" s="8">
         <v>11223344</v>
       </c>
@@ -4717,7 +4791,7 @@
       <c r="D9" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E9" s="33" t="s">
+      <c r="E9" s="34" t="s">
         <v>46</v>
       </c>
       <c r="F9" s="8" t="s">
@@ -4768,7 +4842,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" ht="45" spans="1:22">
+    <row r="10" ht="43.2" spans="1:22">
       <c r="A10" s="8">
         <v>11223344</v>
       </c>
@@ -4781,7 +4855,7 @@
       <c r="D10" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E10" s="33" t="s">
+      <c r="E10" s="34" t="s">
         <v>46</v>
       </c>
       <c r="F10" s="8" t="s">
@@ -4832,7 +4906,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" ht="45" spans="1:22">
+    <row r="11" ht="43.2" spans="1:22">
       <c r="A11" s="8">
         <v>11223344</v>
       </c>
@@ -4845,7 +4919,7 @@
       <c r="D11" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="33" t="s">
+      <c r="E11" s="34" t="s">
         <v>46</v>
       </c>
       <c r="F11" s="8" t="s">
@@ -4896,7 +4970,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" ht="45" spans="1:22">
+    <row r="12" ht="43.2" spans="1:22">
       <c r="A12" s="8">
         <v>11223344</v>
       </c>
@@ -4909,7 +4983,7 @@
       <c r="D12" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E12" s="33" t="s">
+      <c r="E12" s="34" t="s">
         <v>46</v>
       </c>
       <c r="F12" s="8" t="s">
@@ -4956,7 +5030,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" ht="45" spans="1:22">
+    <row r="13" ht="43.2" spans="1:22">
       <c r="A13" s="8">
         <v>11223344</v>
       </c>
@@ -4969,7 +5043,7 @@
       <c r="D13" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="33" t="s">
+      <c r="E13" s="34" t="s">
         <v>46</v>
       </c>
       <c r="F13" s="8" t="s">
@@ -5020,7 +5094,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" ht="45" spans="1:22">
+    <row r="14" ht="43.2" spans="1:22">
       <c r="A14" s="8">
         <v>11223344</v>
       </c>
@@ -5033,7 +5107,7 @@
       <c r="D14" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E14" s="33" t="s">
+      <c r="E14" s="34" t="s">
         <v>46</v>
       </c>
       <c r="F14" s="8" t="s">
@@ -5084,7 +5158,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" ht="60" spans="1:22">
+    <row r="15" ht="57.6" spans="1:22">
       <c r="A15" s="8">
         <v>11223344</v>
       </c>
@@ -5097,7 +5171,7 @@
       <c r="D15" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E15" s="33" t="s">
+      <c r="E15" s="34" t="s">
         <v>46</v>
       </c>
       <c r="F15" s="8" t="s">
@@ -5148,7 +5222,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" ht="45" spans="1:22">
+    <row r="16" ht="43.2" spans="1:22">
       <c r="A16" s="8">
         <v>11223344</v>
       </c>
@@ -5161,7 +5235,7 @@
       <c r="D16" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E16" s="33" t="s">
+      <c r="E16" s="34" t="s">
         <v>46</v>
       </c>
       <c r="F16" s="8" t="s">
@@ -5212,7 +5286,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" ht="45" spans="1:22">
+    <row r="17" ht="43.2" spans="1:22">
       <c r="A17" s="8">
         <v>11223344</v>
       </c>
@@ -5225,7 +5299,7 @@
       <c r="D17" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="33" t="s">
+      <c r="E17" s="34" t="s">
         <v>46</v>
       </c>
       <c r="F17" s="8" t="s">
@@ -5276,7 +5350,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" ht="60" spans="1:22">
+    <row r="18" ht="57.6" spans="1:22">
       <c r="A18" s="8">
         <v>11223344</v>
       </c>
@@ -5289,7 +5363,7 @@
       <c r="D18" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E18" s="33" t="s">
+      <c r="E18" s="34" t="s">
         <v>46</v>
       </c>
       <c r="F18" s="8" t="s">
@@ -5340,7 +5414,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" ht="90" spans="1:22">
+    <row r="19" ht="86.4" spans="1:22">
       <c r="A19" s="8">
         <v>11223344</v>
       </c>
@@ -5353,7 +5427,7 @@
       <c r="D19" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E19" s="33" t="s">
+      <c r="E19" s="34" t="s">
         <v>46</v>
       </c>
       <c r="F19" s="8" t="s">
@@ -5404,7 +5478,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" ht="45" spans="1:22">
+    <row r="20" ht="43.2" spans="1:22">
       <c r="A20" s="8">
         <v>11223344</v>
       </c>
@@ -5417,7 +5491,7 @@
       <c r="D20" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E20" s="33" t="s">
+      <c r="E20" s="34" t="s">
         <v>46</v>
       </c>
       <c r="F20" s="8" t="s">
@@ -5468,7 +5542,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" ht="45" spans="1:22">
+    <row r="21" ht="43.2" spans="1:22">
       <c r="A21" s="8">
         <v>11223344</v>
       </c>
@@ -5481,7 +5555,7 @@
       <c r="D21" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E21" s="33" t="s">
+      <c r="E21" s="34" t="s">
         <v>46</v>
       </c>
       <c r="F21" s="8" t="s">
@@ -5528,7 +5602,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" ht="45" spans="1:22">
+    <row r="22" ht="43.2" spans="1:22">
       <c r="A22" s="8">
         <v>11223344</v>
       </c>
@@ -5541,7 +5615,7 @@
       <c r="D22" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E22" s="33" t="s">
+      <c r="E22" s="34" t="s">
         <v>46</v>
       </c>
       <c r="F22" s="8" t="s">
@@ -5592,7 +5666,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="23" ht="45" spans="1:22">
+    <row r="23" ht="43.2" spans="1:22">
       <c r="A23" s="8">
         <v>11223344</v>
       </c>
@@ -5605,7 +5679,7 @@
       <c r="D23" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E23" s="33" t="s">
+      <c r="E23" s="34" t="s">
         <v>46</v>
       </c>
       <c r="F23" s="8" t="s">
@@ -5656,7 +5730,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="24" ht="45" spans="1:22">
+    <row r="24" ht="43.2" spans="1:22">
       <c r="A24" s="8">
         <v>11223344</v>
       </c>
@@ -5669,7 +5743,7 @@
       <c r="D24" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E24" s="33" t="s">
+      <c r="E24" s="34" t="s">
         <v>46</v>
       </c>
       <c r="F24" s="8" t="s">
@@ -5720,7 +5794,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="25" ht="45" spans="1:22">
+    <row r="25" ht="43.2" spans="1:22">
       <c r="A25" s="8">
         <v>11223344</v>
       </c>
@@ -5733,7 +5807,7 @@
       <c r="D25" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E25" s="33" t="s">
+      <c r="E25" s="34" t="s">
         <v>46</v>
       </c>
       <c r="F25" s="8" t="s">
@@ -5784,7 +5858,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="26" ht="45" spans="1:22">
+    <row r="26" ht="43.2" spans="1:22">
       <c r="A26" s="8">
         <v>11223344</v>
       </c>
@@ -5797,7 +5871,7 @@
       <c r="D26" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E26" s="33" t="s">
+      <c r="E26" s="34" t="s">
         <v>46</v>
       </c>
       <c r="F26" s="8" t="s">
@@ -5848,7 +5922,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="27" ht="45" spans="1:22">
+    <row r="27" ht="43.2" spans="1:22">
       <c r="A27" s="8">
         <v>11223344</v>
       </c>
@@ -5861,7 +5935,7 @@
       <c r="D27" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E27" s="33" t="s">
+      <c r="E27" s="34" t="s">
         <v>46</v>
       </c>
       <c r="F27" s="8" t="s">
@@ -5912,7 +5986,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="28" ht="45" spans="1:22">
+    <row r="28" ht="43.2" spans="1:22">
       <c r="A28" s="8">
         <v>11223344</v>
       </c>
@@ -5925,7 +5999,7 @@
       <c r="D28" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E28" s="33" t="s">
+      <c r="E28" s="34" t="s">
         <v>46</v>
       </c>
       <c r="F28" s="8" t="s">
@@ -5972,7 +6046,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="29" ht="75" spans="1:22">
+    <row r="29" ht="72" spans="1:22">
       <c r="A29" s="8">
         <v>11223344</v>
       </c>
@@ -5985,7 +6059,7 @@
       <c r="D29" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E29" s="33" t="s">
+      <c r="E29" s="34" t="s">
         <v>46</v>
       </c>
       <c r="F29" s="8" t="s">
@@ -6036,7 +6110,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="30" ht="60" spans="1:22">
+    <row r="30" ht="57.6" spans="1:22">
       <c r="A30" s="8">
         <v>11223344</v>
       </c>
@@ -6049,7 +6123,7 @@
       <c r="D30" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E30" s="33" t="s">
+      <c r="E30" s="34" t="s">
         <v>46</v>
       </c>
       <c r="F30" s="8" t="s">
@@ -6104,7 +6178,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" ht="60" spans="1:22">
+    <row r="31" ht="57.6" spans="1:22">
       <c r="A31" s="8">
         <v>11223344</v>
       </c>
@@ -6117,7 +6191,7 @@
       <c r="D31" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E31" s="33" t="s">
+      <c r="E31" s="34" t="s">
         <v>46</v>
       </c>
       <c r="F31" s="8" t="s">
@@ -6210,44 +6284,46 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AH2"/>
+  <dimension ref="A1:AJ2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+    <sheetView topLeftCell="AE1" workbookViewId="0">
+      <selection activeCell="AL15" sqref="AL15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="22.1416666666667" customWidth="1"/>
-    <col min="2" max="2" width="11.2833333333333" customWidth="1"/>
-    <col min="3" max="3" width="14.8583333333333" customWidth="1"/>
-    <col min="4" max="4" width="17.2833333333333" customWidth="1"/>
-    <col min="5" max="6" width="25.7083333333333" customWidth="1"/>
-    <col min="7" max="7" width="24.1416666666667" customWidth="1"/>
-    <col min="8" max="9" width="36.5666666666667" customWidth="1"/>
-    <col min="10" max="10" width="25.5666666666667" customWidth="1"/>
-    <col min="11" max="11" width="36.5666666666667" customWidth="1"/>
-    <col min="12" max="12" width="33.5666666666667" customWidth="1"/>
-    <col min="13" max="13" width="23.1416666666667" customWidth="1"/>
-    <col min="14" max="14" width="35.8583333333333" customWidth="1"/>
-    <col min="15" max="15" width="31.1416666666667" customWidth="1"/>
-    <col min="16" max="16" width="28.5666666666667" customWidth="1"/>
-    <col min="17" max="17" width="26.8583333333333" customWidth="1"/>
-    <col min="18" max="23" width="28.1416666666667" customWidth="1"/>
+    <col min="1" max="1" width="22.1388888888889" customWidth="1"/>
+    <col min="2" max="2" width="11.287037037037" customWidth="1"/>
+    <col min="3" max="3" width="14.8611111111111" customWidth="1"/>
+    <col min="4" max="4" width="17.287037037037" customWidth="1"/>
+    <col min="5" max="6" width="25.712962962963" customWidth="1"/>
+    <col min="7" max="7" width="24.1388888888889" customWidth="1"/>
+    <col min="8" max="9" width="36.5648148148148" customWidth="1"/>
+    <col min="10" max="10" width="25.5648148148148" customWidth="1"/>
+    <col min="11" max="11" width="36.5648148148148" customWidth="1"/>
+    <col min="12" max="12" width="33.5648148148148" customWidth="1"/>
+    <col min="13" max="13" width="23.1388888888889" customWidth="1"/>
+    <col min="14" max="14" width="35.8611111111111" customWidth="1"/>
+    <col min="15" max="15" width="31.1388888888889" customWidth="1"/>
+    <col min="16" max="16" width="28.5648148148148" customWidth="1"/>
+    <col min="17" max="17" width="26.8611111111111" customWidth="1"/>
+    <col min="18" max="23" width="28.1388888888889" customWidth="1"/>
     <col min="24" max="24" width="17" customWidth="1"/>
-    <col min="25" max="25" width="20.5666666666667" customWidth="1"/>
-    <col min="26" max="26" width="25.7083333333333" customWidth="1"/>
-    <col min="27" max="27" width="24.5666666666667" customWidth="1"/>
-    <col min="28" max="28" width="36.5666666666667" customWidth="1"/>
-    <col min="29" max="29" width="33.8583333333333" customWidth="1"/>
-    <col min="30" max="30" width="27.8583333333333" customWidth="1"/>
-    <col min="31" max="31" width="34.5666666666667" customWidth="1"/>
-    <col min="32" max="32" width="35.8583333333333" customWidth="1"/>
+    <col min="25" max="25" width="20.5648148148148" customWidth="1"/>
+    <col min="26" max="26" width="25.712962962963" customWidth="1"/>
+    <col min="27" max="27" width="24.5648148148148" customWidth="1"/>
+    <col min="28" max="28" width="36.5648148148148" customWidth="1"/>
+    <col min="29" max="29" width="33.8611111111111" customWidth="1"/>
+    <col min="30" max="30" width="27.8611111111111" customWidth="1"/>
+    <col min="31" max="31" width="34.5648148148148" customWidth="1"/>
+    <col min="32" max="32" width="35.8611111111111" customWidth="1"/>
     <col min="33" max="33" width="21" customWidth="1"/>
     <col min="34" max="34" width="35" customWidth="1"/>
+    <col min="35" max="35" width="23.4444444444444" customWidth="1"/>
+    <col min="36" max="36" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" spans="1:34">
+    <row r="1" ht="28.8" spans="1:36">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -6350,8 +6426,14 @@
       <c r="AH1" s="8" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="2" ht="30" spans="1:34">
+      <c r="AI1" s="33" t="s">
+        <v>219</v>
+      </c>
+      <c r="AJ1" s="33" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="2" ht="28.8" spans="1:36">
       <c r="A2" s="8">
         <v>11223344</v>
       </c>
@@ -6364,63 +6446,63 @@
       <c r="D2" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E2" s="33" t="s">
+      <c r="E2" s="34" t="s">
         <v>46</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>47</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="M2" s="8">
         <v>405672008</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="O2" s="8" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="P2" s="8" t="s">
         <v>25</v>
       </c>
       <c r="Q2" s="8" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="R2" s="8" t="s">
         <v>19</v>
       </c>
       <c r="S2" s="8" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="T2" s="8" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="U2" s="7" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="V2" s="7" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="W2" s="8"/>
       <c r="X2" s="8" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="Y2" s="8" t="s">
         <v>25</v>
@@ -6429,28 +6511,34 @@
         <v>25</v>
       </c>
       <c r="AA2" s="8" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="AB2" s="7" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="AC2" s="8" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="AD2" s="8" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="AE2" s="8" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="AF2" s="8" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="AG2" s="8">
         <v>1234567890</v>
       </c>
       <c r="AH2" s="8" t="s">
-        <v>239</v>
+        <v>241</v>
+      </c>
+      <c r="AI2" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="AJ2" s="33" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -6466,53 +6554,54 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AO3"/>
+  <dimension ref="A1:AP3"/>
   <sheetViews>
-    <sheetView topLeftCell="AA1" workbookViewId="0">
-      <selection activeCell="AE8" sqref="AE8"/>
+    <sheetView topLeftCell="AL1" workbookViewId="0">
+      <selection activeCell="AR9" sqref="AR9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="2"/>
   <cols>
-    <col min="1" max="1" width="36.5666666666667" customWidth="1"/>
-    <col min="2" max="2" width="23.7083333333333" customWidth="1"/>
-    <col min="3" max="3" width="22.1416666666667" customWidth="1"/>
+    <col min="1" max="1" width="36.5648148148148" customWidth="1"/>
+    <col min="2" max="2" width="23.712962962963" customWidth="1"/>
+    <col min="3" max="3" width="22.1388888888889" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="14.425" customWidth="1"/>
-    <col min="8" max="8" width="26.1416666666667" customWidth="1"/>
-    <col min="9" max="10" width="36.5666666666667" customWidth="1"/>
-    <col min="11" max="11" width="19.7083333333333" customWidth="1"/>
-    <col min="12" max="12" width="32.425" customWidth="1"/>
-    <col min="13" max="13" width="36.5666666666667" customWidth="1"/>
-    <col min="14" max="14" width="20.2833333333333" customWidth="1"/>
+    <col min="7" max="7" width="14.4259259259259" customWidth="1"/>
+    <col min="8" max="8" width="26.1388888888889" customWidth="1"/>
+    <col min="9" max="10" width="36.5648148148148" customWidth="1"/>
+    <col min="11" max="11" width="19.712962962963" customWidth="1"/>
+    <col min="12" max="12" width="32.4259259259259" customWidth="1"/>
+    <col min="13" max="13" width="36.5648148148148" customWidth="1"/>
+    <col min="14" max="14" width="20.287037037037" customWidth="1"/>
     <col min="15" max="15" width="18" customWidth="1"/>
     <col min="16" max="16" width="10" customWidth="1"/>
-    <col min="17" max="17" width="9.28333333333333" customWidth="1"/>
-    <col min="20" max="20" width="12.5666666666667" customWidth="1"/>
-    <col min="21" max="21" width="16.1416666666667" customWidth="1"/>
-    <col min="22" max="22" width="12.7083333333333" customWidth="1"/>
-    <col min="23" max="23" width="11.425" customWidth="1"/>
-    <col min="24" max="24" width="24.1416666666667" customWidth="1"/>
-    <col min="25" max="25" width="29.425" customWidth="1"/>
+    <col min="17" max="17" width="9.28703703703704" customWidth="1"/>
+    <col min="20" max="20" width="12.5648148148148" customWidth="1"/>
+    <col min="21" max="21" width="16.1388888888889" customWidth="1"/>
+    <col min="22" max="22" width="12.7037037037037" customWidth="1"/>
+    <col min="23" max="23" width="11.4259259259259" customWidth="1"/>
+    <col min="24" max="24" width="24.1388888888889" customWidth="1"/>
+    <col min="25" max="25" width="29.4259259259259" customWidth="1"/>
     <col min="26" max="26" width="16" customWidth="1"/>
-    <col min="27" max="27" width="28.7083333333333" customWidth="1"/>
-    <col min="28" max="28" width="30.5666666666667" customWidth="1"/>
-    <col min="29" max="29" width="27.425" customWidth="1"/>
-    <col min="30" max="30" width="34.1416666666667" customWidth="1"/>
-    <col min="31" max="31" width="29.425" customWidth="1"/>
-    <col min="32" max="32" width="23.1416666666667" customWidth="1"/>
+    <col min="27" max="27" width="28.712962962963" customWidth="1"/>
+    <col min="28" max="28" width="30.5648148148148" customWidth="1"/>
+    <col min="29" max="29" width="27.4259259259259" customWidth="1"/>
+    <col min="30" max="30" width="34.1388888888889" customWidth="1"/>
+    <col min="31" max="31" width="29.4259259259259" customWidth="1"/>
+    <col min="32" max="32" width="23.1388888888889" customWidth="1"/>
     <col min="33" max="33" width="36" customWidth="1"/>
-    <col min="34" max="34" width="36.5666666666667" customWidth="1"/>
-    <col min="35" max="35" width="27.8583333333333" customWidth="1"/>
-    <col min="36" max="37" width="36.5666666666667" customWidth="1"/>
-    <col min="38" max="38" width="26.8583333333333" customWidth="1"/>
-    <col min="39" max="40" width="36.5666666666667" customWidth="1"/>
-    <col min="41" max="41" width="23.2833333333333" customWidth="1"/>
+    <col min="34" max="34" width="36.5648148148148" customWidth="1"/>
+    <col min="35" max="35" width="27.8611111111111" customWidth="1"/>
+    <col min="36" max="37" width="36.5648148148148" customWidth="1"/>
+    <col min="38" max="38" width="26.8611111111111" customWidth="1"/>
+    <col min="39" max="40" width="36.5648148148148" customWidth="1"/>
+    <col min="41" max="41" width="23.287037037037" customWidth="1"/>
+    <col min="42" max="42" width="23.3333333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" spans="1:41">
+    <row r="1" ht="28.8" spans="1:42">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -6520,124 +6609,127 @@
         <v>2</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="N1" s="8" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="O1" s="8" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="P1" s="8" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="Q1" s="8" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="R1" s="8" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="S1" s="8" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="T1" s="8" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="U1" s="8" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="V1" s="8" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="W1" s="8" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="X1" s="8" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="Y1" s="8" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="Z1" s="8" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="AA1" s="8" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="AB1" s="8" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="AC1" s="8" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="AD1" s="8" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="AE1" s="8" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="AF1" s="8" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="AG1" s="8" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="AH1" s="8" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="AI1" s="8" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="AJ1" s="7" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="AK1" s="8" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="AL1" s="8" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="AM1" s="7" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="AN1" s="7" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="AO1" s="8" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="2" ht="30" spans="1:41">
+        <v>280</v>
+      </c>
+      <c r="AP1" s="33" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="2" ht="28.8" spans="1:42">
       <c r="A2" s="8">
         <v>11223344</v>
       </c>
@@ -6645,47 +6737,47 @@
         <v>14</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="N2" s="32">
         <v>29783</v>
       </c>
       <c r="O2" s="8" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="P2" s="8"/>
       <c r="Q2" s="8" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="R2" s="8" t="s">
         <v>23</v>
@@ -6694,37 +6786,37 @@
         <v>10032</v>
       </c>
       <c r="T2" s="8" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="U2" s="8">
         <v>1234567890</v>
       </c>
       <c r="V2" s="8" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="W2" s="8" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="X2" s="8" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="Y2" s="8" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="Z2" s="8" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="AA2" s="8" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="AB2" s="8" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="AC2" s="8" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="AD2" s="8" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="AE2" s="8" t="s">
         <v>50</v>
@@ -6733,31 +6825,34 @@
         <v>407376001</v>
       </c>
       <c r="AG2" s="8" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="AH2" s="8" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="AI2" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="AJ2" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="AK2" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="AL2" s="8" t="s">
+        <v>304</v>
+      </c>
+      <c r="AM2" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="AJ2" s="7" t="s">
-        <v>237</v>
-      </c>
-      <c r="AK2" s="8" t="s">
-        <v>238</v>
-      </c>
-      <c r="AL2" s="8" t="s">
-        <v>301</v>
-      </c>
-      <c r="AM2" s="7" t="s">
-        <v>234</v>
-      </c>
       <c r="AN2" s="7" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="AO2" s="8" t="s">
-        <v>303</v>
+        <v>306</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="3" spans="1:1">
@@ -6779,38 +6874,38 @@
       <selection activeCell="C32" sqref="$A1:$XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="32.375" customWidth="1"/>
-    <col min="2" max="2" width="33.875" customWidth="1"/>
-    <col min="3" max="3" width="31.625" customWidth="1"/>
-    <col min="4" max="5" width="36.625" customWidth="1"/>
-    <col min="6" max="6" width="36.875" customWidth="1"/>
-    <col min="7" max="7" width="36.625" customWidth="1"/>
-    <col min="8" max="8" width="17.125" customWidth="1"/>
+    <col min="1" max="1" width="32.3796296296296" customWidth="1"/>
+    <col min="2" max="2" width="33.8796296296296" customWidth="1"/>
+    <col min="3" max="3" width="31.6296296296296" customWidth="1"/>
+    <col min="4" max="5" width="36.6296296296296" customWidth="1"/>
+    <col min="6" max="6" width="36.8796296296296" customWidth="1"/>
+    <col min="7" max="7" width="36.6296296296296" customWidth="1"/>
+    <col min="8" max="8" width="17.1296296296296" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="20" customFormat="1" ht="15.75" spans="1:8">
+    <row r="1" s="20" customFormat="1" ht="15.6" spans="1:8">
       <c r="A1" s="3" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="F1" s="5"/>
       <c r="G1" s="6"/>
       <c r="H1" s="3"/>
     </row>
-    <row r="2" ht="15" spans="1:8">
+    <row r="2" spans="1:8">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
@@ -6818,19 +6913,19 @@
         <v>0</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="D2" s="9" t="b">
         <v>1</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
     </row>
-    <row r="3" ht="15" spans="1:8">
+    <row r="3" spans="1:8">
       <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
@@ -6838,19 +6933,19 @@
         <v>1</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="D3" s="9" t="b">
         <v>1</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
     </row>
-    <row r="4" ht="15" spans="1:8">
+    <row r="4" spans="1:8">
       <c r="A4" s="8" t="s">
         <v>2</v>
       </c>
@@ -6858,19 +6953,19 @@
         <v>2</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="D4" s="9" t="b">
         <v>1</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
     </row>
-    <row r="5" ht="15" spans="1:8">
+    <row r="5" spans="1:8">
       <c r="A5" s="8" t="s">
         <v>4</v>
       </c>
@@ -6878,19 +6973,19 @@
         <v>4</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
     </row>
-    <row r="6" ht="15" spans="1:8">
+    <row r="6" spans="1:8">
       <c r="A6" s="8" t="s">
         <v>3</v>
       </c>
@@ -6898,55 +6993,55 @@
         <v>3</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="30"/>
       <c r="H6" s="8"/>
     </row>
-    <row r="7" ht="15" spans="1:8">
+    <row r="7" spans="1:8">
       <c r="A7" s="12"/>
       <c r="B7" s="12" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
     </row>
-    <row r="8" ht="15" spans="1:8">
+    <row r="8" spans="1:8">
       <c r="A8" s="12"/>
       <c r="B8" s="12" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D8" s="13" t="b">
         <v>1</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
       <c r="H8" s="31"/>
     </row>
-    <row r="9" ht="15" spans="1:8">
+    <row r="9" spans="1:8">
       <c r="A9" s="8" t="s">
         <v>7</v>
       </c>
@@ -6954,37 +7049,37 @@
         <v>7</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
     </row>
-    <row r="10" ht="15" spans="1:8">
+    <row r="10" spans="1:8">
       <c r="A10" s="12"/>
       <c r="B10" s="12" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
     </row>
-    <row r="11" ht="15" spans="1:8">
+    <row r="11" spans="1:8">
       <c r="A11" s="8" t="s">
         <v>9</v>
       </c>
@@ -6992,19 +7087,19 @@
         <v>9</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
     </row>
-    <row r="12" ht="15" spans="1:8">
+    <row r="12" spans="1:8">
       <c r="A12" s="8" t="s">
         <v>10</v>
       </c>
@@ -7012,39 +7107,39 @@
         <v>10</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
     </row>
-    <row r="13" ht="15" spans="1:8">
+    <row r="13" spans="1:8">
       <c r="A13" s="15" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="B13" s="15" t="s">
         <v>12</v>
       </c>
       <c r="C13" s="15" t="s">
+        <v>318</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>314</v>
+      </c>
+      <c r="E13" s="15" t="s">
         <v>315</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>311</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>312</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
     </row>
-    <row r="14" ht="15" spans="1:8">
+    <row r="14" spans="1:8">
       <c r="A14" s="8" t="s">
         <v>11</v>
       </c>
@@ -7052,19 +7147,19 @@
         <v>11</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
     </row>
-    <row r="15" ht="15" spans="1:8">
+    <row r="15" spans="1:8">
       <c r="A15" s="8" t="s">
         <v>13</v>
       </c>
@@ -7072,25 +7167,25 @@
         <v>13</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="D15" s="9" t="b">
         <v>1</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
     </row>
-    <row r="16" ht="15" spans="1:8">
+    <row r="16" spans="1:8">
       <c r="A16" s="18" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="B16" s="18"/>
       <c r="C16" s="18" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="D16" s="19"/>
       <c r="E16" s="18"/>
@@ -7098,13 +7193,13 @@
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
     </row>
-    <row r="17" ht="15" spans="1:8">
+    <row r="17" spans="1:8">
       <c r="A17" s="18" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="B17" s="18"/>
       <c r="C17" s="18" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="D17" s="19"/>
       <c r="E17" s="18"/>
@@ -7112,13 +7207,13 @@
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
     </row>
-    <row r="18" ht="15" spans="1:8">
+    <row r="18" spans="1:8">
       <c r="A18" s="18" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="B18" s="18"/>
       <c r="C18" s="18" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="D18" s="19"/>
       <c r="E18" s="18"/>
@@ -7126,13 +7221,13 @@
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
     </row>
-    <row r="19" ht="15" spans="1:8">
+    <row r="19" spans="1:8">
       <c r="A19" s="18" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="B19" s="18"/>
       <c r="C19" s="18" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="D19" s="19"/>
       <c r="E19" s="17"/>
@@ -7161,38 +7256,38 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="65.875" customWidth="1"/>
-    <col min="2" max="2" width="36.125" customWidth="1"/>
-    <col min="3" max="3" width="26.375" customWidth="1"/>
-    <col min="4" max="4" width="36.625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="65.8796296296296" customWidth="1"/>
+    <col min="2" max="2" width="36.1296296296296" customWidth="1"/>
+    <col min="3" max="3" width="26.3796296296296" customWidth="1"/>
+    <col min="4" max="4" width="36.6296296296296" style="1" customWidth="1"/>
     <col min="5" max="5" width="21.75" customWidth="1"/>
-    <col min="6" max="6" width="37.875" customWidth="1"/>
+    <col min="6" max="6" width="37.8796296296296" customWidth="1"/>
     <col min="7" max="7" width="56.25" customWidth="1"/>
-    <col min="8" max="8" width="42.875" customWidth="1"/>
+    <col min="8" max="8" width="42.8796296296296" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="20" customFormat="1" ht="15.75" spans="1:7">
+    <row r="1" s="20" customFormat="1" ht="15.6" spans="1:7">
       <c r="A1" s="6" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="F1" s="5"/>
       <c r="G1" s="27"/>
     </row>
-    <row r="2" customFormat="1" ht="15" spans="1:6">
+    <row r="2" customFormat="1" spans="1:6">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
@@ -7200,53 +7295,53 @@
         <v>0</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="D2" s="9" t="b">
         <v>1</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F2" s="8"/>
     </row>
-    <row r="3" customFormat="1" ht="15" spans="1:6">
-      <c r="A3" s="34" t="s">
-        <v>324</v>
+    <row r="3" customFormat="1" spans="1:6">
+      <c r="A3" s="35" t="s">
+        <v>327</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D3" s="13" t="b">
         <v>1</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F3" s="8"/>
     </row>
-    <row r="4" customFormat="1" ht="15" spans="1:6">
-      <c r="A4" s="34" t="s">
-        <v>324</v>
+    <row r="4" customFormat="1" spans="1:6">
+      <c r="A4" s="35" t="s">
+        <v>327</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D4" s="13" t="b">
         <v>1</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F4" s="8"/>
     </row>
-    <row r="5" customFormat="1" ht="15" spans="1:6">
+    <row r="5" customFormat="1" spans="1:6">
       <c r="A5" s="8" t="s">
         <v>26</v>
       </c>
@@ -7254,53 +7349,53 @@
         <v>26</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="D5" s="9" t="b">
         <v>1</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F5" s="8"/>
     </row>
-    <row r="6" customFormat="1" ht="15" spans="1:6">
+    <row r="6" customFormat="1" spans="1:6">
       <c r="A6" s="21" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="B6" s="22" t="s">
         <v>27</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D6" s="13" t="b">
         <v>1</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F6" s="8"/>
     </row>
-    <row r="7" customFormat="1" ht="15" spans="1:6">
-      <c r="A7" s="34" t="s">
-        <v>324</v>
+    <row r="7" customFormat="1" spans="1:6">
+      <c r="A7" s="35" t="s">
+        <v>327</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>28</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D7" s="13" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F7" s="8"/>
     </row>
-    <row r="8" customFormat="1" ht="15" spans="1:6">
+    <row r="8" customFormat="1" spans="1:6">
       <c r="A8" s="8" t="s">
         <v>29</v>
       </c>
@@ -7308,17 +7403,17 @@
         <v>29</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="D8" s="9" t="b">
         <v>1</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F8" s="8"/>
     </row>
-    <row r="9" customFormat="1" ht="15" spans="1:6">
+    <row r="9" customFormat="1" spans="1:6">
       <c r="A9" s="8" t="s">
         <v>30</v>
       </c>
@@ -7326,47 +7421,47 @@
         <v>30</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="D9" s="9" t="b">
         <v>1</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F9" s="8"/>
     </row>
-    <row r="10" customFormat="1" ht="15" spans="1:6">
-      <c r="A10" s="34" t="s">
-        <v>324</v>
+    <row r="10" customFormat="1" spans="1:6">
+      <c r="A10" s="35" t="s">
+        <v>327</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>31</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D10" s="13" t="b">
         <v>1</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F10" s="8"/>
     </row>
-    <row r="11" customFormat="1" ht="15" spans="1:6">
+    <row r="11" customFormat="1" spans="1:6">
       <c r="A11" s="18" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="B11" s="18"/>
       <c r="C11" s="18" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="D11" s="19"/>
       <c r="E11" s="18"/>
       <c r="F11" s="8"/>
     </row>
-    <row r="12" customFormat="1" ht="15" spans="1:6">
+    <row r="12" customFormat="1" spans="1:6">
       <c r="A12" s="8" t="s">
         <v>32</v>
       </c>
@@ -7374,67 +7469,67 @@
         <v>32</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="D12" s="9" t="b">
         <v>1</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F12" s="24"/>
     </row>
-    <row r="13" customFormat="1" ht="15" spans="1:6">
+    <row r="13" customFormat="1" spans="1:6">
       <c r="A13" s="15" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="B13" s="15" t="s">
         <v>33</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="D13" s="16" t="b">
         <v>1</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F13" s="8"/>
     </row>
-    <row r="14" customFormat="1" ht="15" spans="1:6">
+    <row r="14" customFormat="1" spans="1:6">
       <c r="A14" s="18" t="s">
+        <v>330</v>
+      </c>
+      <c r="B14" s="36" t="s">
         <v>327</v>
       </c>
-      <c r="B14" s="35" t="s">
-        <v>324</v>
-      </c>
       <c r="C14" s="18" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="D14" s="19"/>
       <c r="E14" s="18"/>
       <c r="F14" s="8"/>
     </row>
-    <row r="15" customFormat="1" ht="15" spans="1:6">
-      <c r="A15" s="34" t="s">
-        <v>324</v>
+    <row r="15" customFormat="1" spans="1:6">
+      <c r="A15" s="35" t="s">
+        <v>327</v>
       </c>
       <c r="B15" s="12" t="s">
         <v>34</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D15" s="13" t="b">
         <v>1</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F15" s="8"/>
     </row>
-    <row r="16" customFormat="1" ht="15" spans="1:7">
+    <row r="16" customFormat="1" spans="1:7">
       <c r="A16" s="8" t="s">
         <v>35</v>
       </c>
@@ -7442,18 +7537,18 @@
         <v>35</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F16" s="8"/>
       <c r="G16" s="28"/>
     </row>
-    <row r="17" customFormat="1" ht="15" spans="1:6">
+    <row r="17" customFormat="1" spans="1:6">
       <c r="A17" s="8" t="s">
         <v>36</v>
       </c>
@@ -7461,35 +7556,35 @@
         <v>36</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F17" s="8"/>
     </row>
-    <row r="18" customFormat="1" ht="15" spans="1:6">
-      <c r="A18" s="34" t="s">
-        <v>324</v>
+    <row r="18" customFormat="1" spans="1:6">
+      <c r="A18" s="35" t="s">
+        <v>327</v>
       </c>
       <c r="B18" s="12" t="s">
         <v>37</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D18" s="13" t="b">
         <v>1</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F18" s="8"/>
     </row>
-    <row r="19" ht="15" spans="1:8">
+    <row r="19" spans="1:8">
       <c r="A19" s="8" t="s">
         <v>39</v>
       </c>
@@ -7497,19 +7592,19 @@
         <v>39</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="D19" s="13" t="b">
         <v>1</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F19" s="8"/>
       <c r="G19" s="26"/>
       <c r="H19" s="26"/>
     </row>
-    <row r="20" customFormat="1" ht="15" spans="1:6">
+    <row r="20" customFormat="1" spans="1:6">
       <c r="A20" s="8" t="s">
         <v>38</v>
       </c>
@@ -7517,59 +7612,59 @@
         <v>38</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="D20" s="9" t="b">
         <v>1</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F20" s="8"/>
     </row>
-    <row r="21" customFormat="1" ht="15" spans="1:6">
+    <row r="21" customFormat="1" spans="1:6">
       <c r="A21" s="18" t="s">
-        <v>328</v>
-      </c>
-      <c r="B21" s="35" t="s">
-        <v>324</v>
+        <v>331</v>
+      </c>
+      <c r="B21" s="36" t="s">
+        <v>327</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="D21" s="19"/>
       <c r="E21" s="18"/>
       <c r="F21" s="8"/>
     </row>
-    <row r="22" customFormat="1" ht="15" spans="1:6">
+    <row r="22" customFormat="1" spans="1:6">
       <c r="A22" s="18" t="s">
-        <v>329</v>
-      </c>
-      <c r="B22" s="35" t="s">
-        <v>324</v>
+        <v>332</v>
+      </c>
+      <c r="B22" s="36" t="s">
+        <v>327</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="D22" s="19"/>
       <c r="E22" s="18"/>
       <c r="F22" s="8"/>
     </row>
-    <row r="23" customFormat="1" ht="15" spans="1:6">
+    <row r="23" customFormat="1" spans="1:6">
       <c r="A23" s="18" t="s">
-        <v>330</v>
-      </c>
-      <c r="B23" s="35" t="s">
-        <v>324</v>
+        <v>333</v>
+      </c>
+      <c r="B23" s="36" t="s">
+        <v>327</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="D23" s="19"/>
       <c r="E23" s="18"/>
       <c r="F23" s="8"/>
     </row>
-    <row r="24" customFormat="1" ht="15" spans="1:6">
+    <row r="24" customFormat="1" spans="1:6">
       <c r="A24" s="8" t="s">
         <v>40</v>
       </c>
@@ -7577,17 +7672,17 @@
         <v>40</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F24" s="8"/>
     </row>
-    <row r="25" customFormat="1" ht="15" spans="1:6">
+    <row r="25" customFormat="1" spans="1:6">
       <c r="A25" s="8" t="s">
         <v>41</v>
       </c>
@@ -7595,77 +7690,77 @@
         <v>41</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F25" s="8"/>
     </row>
-    <row r="26" customFormat="1" ht="15" spans="1:6">
+    <row r="26" customFormat="1" spans="1:6">
       <c r="A26" s="18" t="s">
-        <v>331</v>
-      </c>
-      <c r="B26" s="35" t="s">
-        <v>324</v>
+        <v>334</v>
+      </c>
+      <c r="B26" s="36" t="s">
+        <v>327</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="D26" s="19"/>
       <c r="E26" s="18"/>
       <c r="F26" s="8"/>
     </row>
-    <row r="27" customFormat="1" ht="15" spans="1:6">
-      <c r="A27" s="34" t="s">
-        <v>324</v>
+    <row r="27" customFormat="1" spans="1:6">
+      <c r="A27" s="35" t="s">
+        <v>327</v>
       </c>
       <c r="B27" s="12" t="s">
         <v>42</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D27" s="13" t="b">
         <v>1</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F27" s="8"/>
     </row>
-    <row r="28" customFormat="1" ht="15" spans="1:6">
+    <row r="28" customFormat="1" spans="1:6">
       <c r="A28" s="12"/>
       <c r="B28" s="29" t="s">
         <v>43</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D28" s="13" t="b">
         <v>1</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F28" s="8"/>
     </row>
-    <row r="29" customFormat="1" ht="15" spans="1:6">
+    <row r="29" customFormat="1" spans="1:6">
       <c r="A29" s="12"/>
       <c r="B29" s="23" t="s">
         <v>44</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F29" s="8"/>
     </row>
@@ -7678,17 +7773,17 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="41.625" customWidth="1"/>
+    <col min="1" max="1" width="41.6296296296296" customWidth="1"/>
     <col min="2" max="2" width="47.25" customWidth="1"/>
-    <col min="3" max="3" width="14.875" customWidth="1"/>
+    <col min="3" max="3" width="14.8796296296296" customWidth="1"/>
     <col min="4" max="4" width="26.25" style="1" customWidth="1"/>
     <col min="5" max="5" width="24.25" customWidth="1"/>
     <col min="6" max="6" width="37.25" customWidth="1"/>
@@ -7696,26 +7791,26 @@
     <col min="8" max="8" width="44.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="20" customFormat="1" ht="15.75" spans="1:7">
+    <row r="1" s="20" customFormat="1" ht="15.6" spans="1:7">
       <c r="A1" s="3" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="F1" s="5"/>
       <c r="G1" s="6"/>
     </row>
-    <row r="2" customFormat="1" ht="15" spans="1:7">
+    <row r="2" customFormat="1" spans="1:7">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
@@ -7723,52 +7818,52 @@
         <v>0</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="D2" s="9" t="b">
         <v>1</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
     </row>
-    <row r="3" customFormat="1" ht="15" spans="1:7">
+    <row r="3" customFormat="1" spans="1:7">
       <c r="A3" s="12"/>
       <c r="B3" s="12" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D3" s="13" t="b">
         <v>1</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
     </row>
-    <row r="4" customFormat="1" ht="15" spans="1:7">
+    <row r="4" customFormat="1" spans="1:7">
       <c r="A4" s="12"/>
       <c r="B4" s="12" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D4" s="13" t="b">
         <v>1</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
     </row>
-    <row r="5" customFormat="1" ht="15" spans="1:7">
+    <row r="5" customFormat="1" spans="1:7">
       <c r="A5" s="8" t="s">
         <v>26</v>
       </c>
@@ -7776,53 +7871,53 @@
         <v>26</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="D5" s="9" t="b">
         <v>1</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
     </row>
-    <row r="6" customFormat="1" ht="15" spans="1:6">
+    <row r="6" customFormat="1" spans="1:6">
       <c r="A6" s="21" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="B6" s="22" t="s">
         <v>27</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D6" s="13" t="b">
         <v>1</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F6" s="8"/>
     </row>
-    <row r="7" customFormat="1" ht="15" spans="1:7">
+    <row r="7" customFormat="1" spans="1:7">
       <c r="A7" s="12"/>
       <c r="B7" s="12" t="s">
         <v>28</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D7" s="13" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
     </row>
-    <row r="8" customFormat="1" ht="15" spans="1:7">
+    <row r="8" customFormat="1" spans="1:7">
       <c r="A8" s="8" t="s">
         <v>192</v>
       </c>
@@ -7830,52 +7925,52 @@
         <v>192</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="D8" s="9" t="b">
         <v>1</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
     </row>
-    <row r="9" customFormat="1" ht="15" spans="1:7">
+    <row r="9" customFormat="1" spans="1:7">
       <c r="A9" s="12"/>
       <c r="B9" s="12" t="s">
         <v>194</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D9" s="13" t="b">
         <v>1</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
     </row>
-    <row r="10" customFormat="1" ht="15" spans="1:7">
+    <row r="10" customFormat="1" spans="1:7">
       <c r="A10" s="12"/>
       <c r="B10" s="12" t="s">
         <v>193</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D10" s="13" t="b">
         <v>1</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
     </row>
-    <row r="11" customFormat="1" ht="15" spans="1:7">
+    <row r="11" customFormat="1" spans="1:7">
       <c r="A11" s="8" t="s">
         <v>195</v>
       </c>
@@ -7883,52 +7978,52 @@
         <v>195</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="D11" s="9" t="b">
         <v>1</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
     </row>
-    <row r="12" customFormat="1" ht="15" spans="1:7">
+    <row r="12" customFormat="1" spans="1:7">
       <c r="A12" s="12"/>
       <c r="B12" s="12" t="s">
         <v>197</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D12" s="13" t="b">
         <v>1</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
     </row>
-    <row r="13" customFormat="1" ht="15" spans="1:7">
+    <row r="13" customFormat="1" spans="1:7">
       <c r="A13" s="12"/>
       <c r="B13" s="12" t="s">
         <v>196</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D13" s="13" t="b">
         <v>1</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
     </row>
-    <row r="14" customFormat="1" ht="15" spans="1:7">
+    <row r="14" customFormat="1" spans="1:7">
       <c r="A14" s="8" t="s">
         <v>198</v>
       </c>
@@ -7936,18 +8031,18 @@
         <v>198</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="D14" s="9" t="b">
         <v>1</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
     </row>
-    <row r="15" customFormat="1" ht="15" spans="1:7">
+    <row r="15" customFormat="1" spans="1:7">
       <c r="A15" s="8" t="s">
         <v>199</v>
       </c>
@@ -7955,18 +8050,18 @@
         <v>199</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
     </row>
-    <row r="16" customFormat="1" ht="15" spans="1:7">
+    <row r="16" customFormat="1" spans="1:7">
       <c r="A16" s="8" t="s">
         <v>200</v>
       </c>
@@ -7974,154 +8069,154 @@
         <v>200</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
     </row>
-    <row r="17" customFormat="1" ht="15" spans="1:7">
+    <row r="17" customFormat="1" spans="1:7">
       <c r="A17" s="12"/>
       <c r="B17" s="12" t="s">
         <v>201</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D17" s="13" t="b">
         <v>1</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
     </row>
-    <row r="18" customFormat="1" ht="15" spans="1:7">
+    <row r="18" customFormat="1" spans="1:7">
       <c r="A18" s="12"/>
       <c r="B18" s="12" t="s">
         <v>202</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
     </row>
-    <row r="19" customFormat="1" ht="15" spans="1:7">
+    <row r="19" customFormat="1" spans="1:7">
       <c r="A19" s="12"/>
       <c r="B19" s="12" t="s">
         <v>6</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D19" s="13" t="b">
         <v>1</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
     </row>
-    <row r="20" customFormat="1" ht="15" spans="1:7">
+    <row r="20" customFormat="1" spans="1:7">
       <c r="A20" s="12"/>
       <c r="B20" s="23" t="s">
         <v>203</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
     </row>
-    <row r="21" customFormat="1" ht="15" spans="1:7">
+    <row r="21" customFormat="1" spans="1:7">
       <c r="A21" s="12"/>
       <c r="B21" s="23" t="s">
         <v>205</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
     </row>
-    <row r="22" customFormat="1" ht="15" spans="1:7">
+    <row r="22" customFormat="1" spans="1:7">
       <c r="A22" s="12"/>
       <c r="B22" s="23" t="s">
         <v>204</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F22" s="24"/>
       <c r="G22" s="8"/>
     </row>
-    <row r="23" customFormat="1" ht="15" spans="1:7">
+    <row r="23" customFormat="1" spans="1:7">
       <c r="A23" s="12"/>
       <c r="B23" s="23" t="s">
         <v>206</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
     </row>
-    <row r="24" customFormat="1" ht="15" spans="1:7">
+    <row r="24" customFormat="1" spans="1:7">
       <c r="A24" s="12"/>
       <c r="B24" s="23" t="s">
         <v>207</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
     </row>
-    <row r="25" customFormat="1" ht="15" spans="1:7">
+    <row r="25" customFormat="1" spans="1:7">
       <c r="A25" s="8" t="s">
         <v>208</v>
       </c>
@@ -8129,18 +8224,18 @@
         <v>208</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="D25" s="9" t="b">
         <v>1</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
     </row>
-    <row r="26" customFormat="1" ht="15" spans="1:7">
+    <row r="26" customFormat="1" spans="1:7">
       <c r="A26" s="8" t="s">
         <v>209</v>
       </c>
@@ -8148,57 +8243,57 @@
         <v>209</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="D26" s="9" t="b">
         <v>1</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F26" s="8"/>
       <c r="G26" s="8"/>
     </row>
-    <row r="27" customFormat="1" ht="15" spans="1:7">
+    <row r="27" customFormat="1" spans="1:7">
       <c r="A27" s="18" t="s">
-        <v>332</v>
+        <v>219</v>
       </c>
       <c r="B27" s="18"/>
       <c r="C27" s="18" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="D27" s="19"/>
       <c r="E27" s="18"/>
       <c r="F27" s="8"/>
       <c r="G27" s="8"/>
     </row>
-    <row r="28" customFormat="1" ht="15" spans="1:7">
+    <row r="28" customFormat="1" spans="1:7">
       <c r="A28" s="18" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="B28" s="18"/>
       <c r="C28" s="18" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="D28" s="19"/>
       <c r="E28" s="18"/>
       <c r="F28" s="8"/>
       <c r="G28" s="8"/>
     </row>
-    <row r="29" customFormat="1" ht="15" spans="1:7">
+    <row r="29" customFormat="1" spans="1:7">
       <c r="A29" s="18" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="B29" s="18"/>
       <c r="C29" s="18" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="D29" s="19"/>
       <c r="E29" s="18"/>
       <c r="F29" s="8"/>
       <c r="G29" s="8"/>
     </row>
-    <row r="30" customFormat="1" ht="15" spans="1:7">
+    <row r="30" customFormat="1" spans="1:7">
       <c r="A30" s="8" t="s">
         <v>210</v>
       </c>
@@ -8206,18 +8301,18 @@
         <v>210</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F30" s="8"/>
       <c r="G30" s="8"/>
     </row>
-    <row r="31" ht="15" spans="1:8">
+    <row r="31" spans="1:8">
       <c r="A31" s="8" t="s">
         <v>211</v>
       </c>
@@ -8225,158 +8320,183 @@
         <v>211</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="D31" s="9" t="b">
         <v>1</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F31" s="8"/>
       <c r="G31" s="25"/>
       <c r="H31" s="26"/>
     </row>
-    <row r="32" customFormat="1" ht="15" spans="1:7">
+    <row r="32" customFormat="1" spans="1:7">
       <c r="A32" s="12"/>
       <c r="B32" s="12" t="s">
         <v>212</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D32" s="13" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F32" s="8"/>
       <c r="G32" s="8"/>
     </row>
-    <row r="33" customFormat="1" ht="15" spans="1:7">
+    <row r="33" customFormat="1" spans="1:7">
       <c r="A33" s="12"/>
       <c r="B33" s="12" t="s">
         <v>213</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D33" s="13" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F33" s="8"/>
       <c r="G33" s="8"/>
     </row>
-    <row r="34" customFormat="1" ht="15" spans="1:7">
+    <row r="34" customFormat="1" spans="1:7">
       <c r="A34" s="12"/>
       <c r="B34" s="12" t="s">
         <v>215</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D34" s="13" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F34" s="8"/>
       <c r="G34" s="8"/>
     </row>
-    <row r="35" customFormat="1" ht="15" spans="1:7">
+    <row r="35" customFormat="1" spans="1:7">
       <c r="A35" s="12"/>
       <c r="B35" s="12" t="s">
         <v>214</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D35" s="13" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F35" s="8"/>
       <c r="G35" s="8"/>
     </row>
-    <row r="36" customFormat="1" ht="15" spans="1:7">
+    <row r="36" customFormat="1" spans="1:7">
       <c r="A36" s="12"/>
       <c r="B36" s="12" t="s">
         <v>216</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D36" s="13" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F36" s="8"/>
       <c r="G36" s="8"/>
     </row>
-    <row r="37" customFormat="1" ht="15" spans="1:7">
+    <row r="37" customFormat="1" spans="1:7">
       <c r="A37" s="12"/>
       <c r="B37" s="12" t="s">
         <v>217</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D37" s="13" t="b">
         <v>1</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F37" s="8"/>
       <c r="G37" s="8"/>
     </row>
-    <row r="38" customFormat="1" ht="15" spans="1:7">
+    <row r="38" customFormat="1" spans="1:7">
       <c r="A38" s="12"/>
       <c r="B38" s="12" t="s">
         <v>218</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D38" s="13" t="b">
         <v>1</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F38" s="8"/>
       <c r="G38" s="8"/>
     </row>
-    <row r="39" customFormat="1" ht="15" spans="1:7">
+    <row r="39" customFormat="1" spans="1:7">
       <c r="A39" s="18" t="s">
-        <v>335</v>
+        <v>220</v>
       </c>
       <c r="B39" s="18"/>
       <c r="C39" s="18" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="D39" s="19"/>
       <c r="E39" s="18"/>
       <c r="F39" s="8"/>
       <c r="G39" s="8"/>
     </row>
-    <row r="40" customFormat="1" ht="15" spans="1:7">
-      <c r="A40" s="8"/>
-      <c r="B40" s="8"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="9"/>
-      <c r="E40" s="8"/>
+    <row r="40" customFormat="1" spans="1:7">
+      <c r="A40" s="11"/>
+      <c r="B40" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="D40" s="13" t="s">
+        <v>314</v>
+      </c>
+      <c r="E40" s="12" t="s">
+        <v>315</v>
+      </c>
       <c r="F40" s="8"/>
       <c r="G40" s="8"/>
+    </row>
+    <row r="41" customFormat="1" spans="1:7">
+      <c r="A41" s="11"/>
+      <c r="B41" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="D41" s="13" t="s">
+        <v>314</v>
+      </c>
+      <c r="E41" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8387,40 +8507,40 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A49" sqref="$A49:$XFD49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="30" defaultRowHeight="14.25" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="30" defaultRowHeight="14.4" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="48" customWidth="1"/>
-    <col min="2" max="2" width="36.5666666666667" customWidth="1"/>
+    <col min="2" max="2" width="36.5648148148148" customWidth="1"/>
     <col min="4" max="4" width="30" style="1"/>
-    <col min="6" max="6" width="39.1416666666667" customWidth="1"/>
+    <col min="6" max="6" width="39.1388888888889" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" spans="1:7">
+    <row r="1" ht="15.6" spans="1:7">
       <c r="A1" s="2" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="F1" s="5"/>
       <c r="G1" s="6"/>
     </row>
-    <row r="2" ht="15" spans="1:7">
+    <row r="2" spans="1:7">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
@@ -8428,838 +8548,855 @@
         <v>0</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="D2" s="9" t="b">
         <v>1</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
     </row>
-    <row r="3" ht="15" spans="1:7">
+    <row r="3" spans="1:7">
       <c r="A3" s="11"/>
       <c r="B3" s="11" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D3" s="13" t="b">
         <v>1</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
     </row>
-    <row r="4" ht="15" spans="1:7">
+    <row r="4" spans="1:7">
       <c r="A4" s="14" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="D4" s="16" t="b">
         <v>1</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
     </row>
-    <row r="5" ht="15" spans="1:7">
+    <row r="5" spans="1:7">
       <c r="A5" s="7" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
     </row>
-    <row r="6" ht="15" spans="1:7">
+    <row r="6" spans="1:7">
       <c r="A6" s="7" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="D6" s="9" t="b">
         <v>1</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
     </row>
-    <row r="7" ht="15" spans="1:7">
+    <row r="7" spans="1:7">
       <c r="A7" s="7" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
     </row>
-    <row r="8" ht="15" spans="1:7">
+    <row r="8" spans="1:7">
       <c r="A8" s="7" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="D8" s="9" t="b">
         <v>1</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
     </row>
-    <row r="9" ht="15" spans="1:7">
+    <row r="9" spans="1:7">
       <c r="A9" s="14" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="D9" s="16" t="b">
         <v>1</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
     </row>
-    <row r="10" ht="28.5" spans="1:7">
+    <row r="10" spans="1:7">
       <c r="A10" s="11"/>
       <c r="B10" s="11" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D10" s="13" t="b">
         <v>1</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
     </row>
-    <row r="11" ht="15" spans="1:7">
+    <row r="11" spans="1:7">
       <c r="A11" s="11"/>
       <c r="B11" s="11" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D11" s="13" t="b">
         <v>1</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
     </row>
-    <row r="12" ht="15" spans="1:7">
+    <row r="12" spans="1:7">
       <c r="A12" s="14" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="C12" s="15" t="s">
+        <v>318</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>314</v>
+      </c>
+      <c r="E12" s="15" t="s">
         <v>315</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>311</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>312</v>
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
     </row>
-    <row r="13" ht="15" spans="1:7">
+    <row r="13" spans="1:7">
       <c r="A13" s="11"/>
       <c r="B13" s="11" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
     </row>
-    <row r="14" ht="15" spans="1:7">
+    <row r="14" spans="1:7">
       <c r="A14" s="11"/>
       <c r="B14" s="11" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
     </row>
-    <row r="15" ht="15" spans="1:7">
+    <row r="15" spans="1:7">
       <c r="A15" s="7" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="D15" s="9" t="b">
         <v>1</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
     </row>
-    <row r="16" ht="15" spans="1:7">
+    <row r="16" spans="1:7">
       <c r="A16" s="7" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="D16" s="9" t="b">
         <v>1</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
     </row>
-    <row r="17" ht="15" spans="1:7">
+    <row r="17" spans="1:7">
       <c r="A17" s="11"/>
       <c r="B17" s="11" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
     </row>
-    <row r="18" ht="15" spans="1:7">
+    <row r="18" spans="1:7">
       <c r="A18" s="7" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="D18" s="9" t="b">
         <v>1</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
     </row>
-    <row r="19" ht="15" spans="1:7">
+    <row r="19" spans="1:7">
       <c r="A19" s="14" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="D19" s="16" t="b">
         <v>1</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
     </row>
-    <row r="20" ht="15" spans="1:7">
+    <row r="20" spans="1:7">
       <c r="A20" s="7" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="D20" s="9" t="b">
         <v>1</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
     </row>
-    <row r="21" ht="15" spans="1:7">
+    <row r="21" spans="1:7">
       <c r="A21" s="7" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="D21" s="9" t="b">
         <v>1</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
     </row>
-    <row r="22" ht="15" spans="1:7">
+    <row r="22" spans="1:7">
       <c r="A22" s="7" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
     </row>
-    <row r="23" ht="15" spans="1:7">
+    <row r="23" spans="1:7">
       <c r="A23" s="11"/>
       <c r="B23" s="11" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
     </row>
-    <row r="24" ht="15" spans="1:7">
+    <row r="24" spans="1:7">
       <c r="A24" s="14" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="C24" s="15" t="s">
+        <v>318</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>314</v>
+      </c>
+      <c r="E24" s="15" t="s">
         <v>315</v>
-      </c>
-      <c r="D24" s="16" t="s">
-        <v>311</v>
-      </c>
-      <c r="E24" s="15" t="s">
-        <v>312</v>
       </c>
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
     </row>
-    <row r="25" ht="15" spans="1:7">
+    <row r="25" spans="1:7">
       <c r="A25" s="14" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="C25" s="15" t="s">
+        <v>318</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>314</v>
+      </c>
+      <c r="E25" s="15" t="s">
         <v>315</v>
-      </c>
-      <c r="D25" s="16" t="s">
-        <v>311</v>
-      </c>
-      <c r="E25" s="15" t="s">
-        <v>312</v>
       </c>
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
     </row>
-    <row r="26" ht="15" spans="1:7">
+    <row r="26" spans="1:7">
       <c r="A26" s="14" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="C26" s="15" t="s">
+        <v>318</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>314</v>
+      </c>
+      <c r="E26" s="15" t="s">
         <v>315</v>
-      </c>
-      <c r="D26" s="16" t="s">
-        <v>311</v>
-      </c>
-      <c r="E26" s="15" t="s">
-        <v>312</v>
       </c>
       <c r="F26" s="8"/>
       <c r="G26" s="8"/>
     </row>
-    <row r="27" ht="15" spans="1:7">
+    <row r="27" spans="1:7">
       <c r="A27" s="14" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="C27" s="15" t="s">
+        <v>318</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>314</v>
+      </c>
+      <c r="E27" s="15" t="s">
         <v>315</v>
-      </c>
-      <c r="D27" s="16" t="s">
-        <v>311</v>
-      </c>
-      <c r="E27" s="15" t="s">
-        <v>312</v>
       </c>
       <c r="F27" s="8"/>
       <c r="G27" s="8"/>
     </row>
-    <row r="28" ht="28.5" spans="1:7">
+    <row r="28" spans="1:7">
       <c r="A28" s="14" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="C28" s="15" t="s">
+        <v>318</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>314</v>
+      </c>
+      <c r="E28" s="15" t="s">
         <v>315</v>
-      </c>
-      <c r="D28" s="16" t="s">
-        <v>311</v>
-      </c>
-      <c r="E28" s="15" t="s">
-        <v>312</v>
       </c>
       <c r="F28" s="8"/>
       <c r="G28" s="8"/>
     </row>
-    <row r="29" ht="15" spans="1:7">
+    <row r="29" spans="1:7">
       <c r="A29" s="14" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="C29" s="15" t="s">
+        <v>318</v>
+      </c>
+      <c r="D29" s="16" t="s">
+        <v>314</v>
+      </c>
+      <c r="E29" s="15" t="s">
         <v>315</v>
-      </c>
-      <c r="D29" s="16" t="s">
-        <v>311</v>
-      </c>
-      <c r="E29" s="15" t="s">
-        <v>312</v>
       </c>
       <c r="F29" s="8"/>
       <c r="G29" s="8"/>
     </row>
-    <row r="30" ht="28.5" spans="1:7">
+    <row r="30" spans="1:7">
       <c r="A30" s="14" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="C30" s="15" t="s">
+        <v>318</v>
+      </c>
+      <c r="D30" s="16" t="s">
+        <v>314</v>
+      </c>
+      <c r="E30" s="15" t="s">
         <v>315</v>
-      </c>
-      <c r="D30" s="16" t="s">
-        <v>311</v>
-      </c>
-      <c r="E30" s="15" t="s">
-        <v>312</v>
       </c>
       <c r="F30" s="8"/>
       <c r="G30" s="8"/>
     </row>
-    <row r="31" ht="15" spans="1:7">
+    <row r="31" spans="1:7">
       <c r="A31" s="14" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="C31" s="15" t="s">
+        <v>318</v>
+      </c>
+      <c r="D31" s="16" t="s">
+        <v>314</v>
+      </c>
+      <c r="E31" s="15" t="s">
         <v>315</v>
-      </c>
-      <c r="D31" s="16" t="s">
-        <v>311</v>
-      </c>
-      <c r="E31" s="15" t="s">
-        <v>312</v>
       </c>
       <c r="F31" s="8"/>
       <c r="G31" s="8"/>
     </row>
-    <row r="32" ht="28.5" spans="1:7">
+    <row r="32" spans="1:7">
       <c r="A32" s="11"/>
       <c r="B32" s="11" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D32" s="13" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F32" s="8"/>
       <c r="G32" s="8"/>
     </row>
-    <row r="33" ht="15" spans="1:7">
+    <row r="33" spans="1:7">
       <c r="A33" s="14" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B33" s="14" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C33" s="15" t="s">
+        <v>318</v>
+      </c>
+      <c r="D33" s="16" t="s">
+        <v>314</v>
+      </c>
+      <c r="E33" s="15" t="s">
         <v>315</v>
-      </c>
-      <c r="D33" s="16" t="s">
-        <v>311</v>
-      </c>
-      <c r="E33" s="15" t="s">
-        <v>312</v>
       </c>
       <c r="F33" s="8"/>
       <c r="G33" s="8"/>
     </row>
-    <row r="34" ht="28.5" spans="1:7">
+    <row r="34" spans="1:7">
       <c r="A34" s="14" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="C34" s="15" t="s">
+        <v>318</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>314</v>
+      </c>
+      <c r="E34" s="15" t="s">
         <v>315</v>
-      </c>
-      <c r="D34" s="16" t="s">
-        <v>311</v>
-      </c>
-      <c r="E34" s="15" t="s">
-        <v>312</v>
       </c>
       <c r="F34" s="8"/>
       <c r="G34" s="8"/>
     </row>
-    <row r="35" ht="28.5" spans="1:7">
+    <row r="35" spans="1:7">
       <c r="A35" s="14" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="C35" s="15" t="s">
+        <v>318</v>
+      </c>
+      <c r="D35" s="16" t="s">
+        <v>314</v>
+      </c>
+      <c r="E35" s="15" t="s">
         <v>315</v>
-      </c>
-      <c r="D35" s="16" t="s">
-        <v>311</v>
-      </c>
-      <c r="E35" s="15" t="s">
-        <v>312</v>
       </c>
       <c r="F35" s="8"/>
       <c r="G35" s="8"/>
     </row>
-    <row r="36" ht="15" spans="1:7">
+    <row r="36" spans="1:7">
       <c r="A36" s="14" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B36" s="14" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C36" s="15" t="s">
+        <v>318</v>
+      </c>
+      <c r="D36" s="16" t="s">
+        <v>314</v>
+      </c>
+      <c r="E36" s="15" t="s">
         <v>315</v>
-      </c>
-      <c r="D36" s="16" t="s">
-        <v>311</v>
-      </c>
-      <c r="E36" s="15" t="s">
-        <v>312</v>
       </c>
       <c r="F36" s="8"/>
       <c r="G36" s="8"/>
     </row>
-    <row r="37" ht="28.5" spans="1:7">
+    <row r="37" ht="28.8" spans="1:7">
       <c r="A37" s="14" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="C37" s="15" t="s">
+        <v>318</v>
+      </c>
+      <c r="D37" s="16" t="s">
+        <v>314</v>
+      </c>
+      <c r="E37" s="15" t="s">
         <v>315</v>
-      </c>
-      <c r="D37" s="16" t="s">
-        <v>311</v>
-      </c>
-      <c r="E37" s="15" t="s">
-        <v>312</v>
       </c>
       <c r="F37" s="8"/>
       <c r="G37" s="8"/>
     </row>
-    <row r="38" ht="28.5" spans="1:7">
+    <row r="38" ht="28.8" spans="1:7">
       <c r="A38" s="14" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="C38" s="15" t="s">
+        <v>318</v>
+      </c>
+      <c r="D38" s="16" t="s">
+        <v>314</v>
+      </c>
+      <c r="E38" s="15" t="s">
         <v>315</v>
-      </c>
-      <c r="D38" s="16" t="s">
-        <v>311</v>
-      </c>
-      <c r="E38" s="15" t="s">
-        <v>312</v>
       </c>
       <c r="F38" s="8"/>
       <c r="G38" s="8"/>
     </row>
-    <row r="39" ht="15" spans="1:7">
+    <row r="39" spans="1:7">
       <c r="A39" s="7" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F39" s="8"/>
       <c r="G39" s="8"/>
     </row>
-    <row r="40" ht="15" spans="1:7">
+    <row r="40" spans="1:7">
       <c r="A40" s="17" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B40" s="17"/>
       <c r="C40" s="18" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="D40" s="19"/>
       <c r="E40" s="18"/>
       <c r="F40" s="8"/>
       <c r="G40" s="8"/>
     </row>
-    <row r="41" ht="15" spans="1:7">
+    <row r="41" spans="1:7">
       <c r="A41" s="17" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B41" s="17"/>
       <c r="C41" s="18" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="D41" s="19"/>
       <c r="E41" s="18"/>
       <c r="F41" s="8"/>
       <c r="G41" s="8"/>
     </row>
-    <row r="42" ht="15" spans="1:7">
+    <row r="42" spans="1:7">
       <c r="A42" s="17" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B42" s="17"/>
       <c r="C42" s="18" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="D42" s="19"/>
       <c r="E42" s="18"/>
       <c r="F42" s="8"/>
       <c r="G42" s="8"/>
     </row>
-    <row r="43" ht="15" spans="1:7">
+    <row r="43" spans="1:7">
       <c r="A43" s="17" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B43" s="17"/>
       <c r="C43" s="18" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="D43" s="19"/>
       <c r="E43" s="18"/>
       <c r="F43" s="8"/>
       <c r="G43" s="8"/>
     </row>
-    <row r="44" ht="15" spans="1:7">
+    <row r="44" spans="1:7">
       <c r="A44" s="17" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="B44" s="17"/>
       <c r="C44" s="18" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="D44" s="19"/>
       <c r="E44" s="18"/>
       <c r="F44" s="8"/>
       <c r="G44" s="8"/>
     </row>
-    <row r="45" ht="15" spans="1:7">
+    <row r="45" spans="1:7">
       <c r="A45" s="14" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="B45" s="14" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="C45" s="15" t="s">
+        <v>318</v>
+      </c>
+      <c r="D45" s="16" t="s">
+        <v>314</v>
+      </c>
+      <c r="E45" s="15" t="s">
         <v>315</v>
-      </c>
-      <c r="D45" s="16" t="s">
-        <v>311</v>
-      </c>
-      <c r="E45" s="15" t="s">
-        <v>312</v>
       </c>
       <c r="F45" s="8"/>
       <c r="G45" s="8"/>
     </row>
-    <row r="46" ht="28.5" spans="1:7">
+    <row r="46" spans="1:7">
       <c r="A46" s="14" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="C46" s="15" t="s">
+        <v>318</v>
+      </c>
+      <c r="D46" s="16" t="s">
+        <v>314</v>
+      </c>
+      <c r="E46" s="15" t="s">
         <v>315</v>
-      </c>
-      <c r="D46" s="16" t="s">
-        <v>311</v>
-      </c>
-      <c r="E46" s="15" t="s">
-        <v>312</v>
       </c>
       <c r="F46" s="8"/>
       <c r="G46" s="8"/>
     </row>
-    <row r="47" ht="28.5" spans="1:7">
+    <row r="47" spans="1:7">
       <c r="A47" s="14" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B47" s="14" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="C47" s="15" t="s">
+        <v>318</v>
+      </c>
+      <c r="D47" s="16" t="s">
+        <v>314</v>
+      </c>
+      <c r="E47" s="15" t="s">
         <v>315</v>
-      </c>
-      <c r="D47" s="16" t="s">
-        <v>311</v>
-      </c>
-      <c r="E47" s="15" t="s">
-        <v>312</v>
       </c>
       <c r="F47" s="8"/>
       <c r="G47" s="8"/>
     </row>
-    <row r="48" ht="15" spans="1:7">
+    <row r="48" spans="1:7">
       <c r="A48" s="17" t="s">
-        <v>362</v>
+        <v>281</v>
       </c>
       <c r="B48" s="17"/>
       <c r="C48" s="18" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="D48" s="19"/>
       <c r="E48" s="18"/>
       <c r="F48" s="8"/>
       <c r="G48" s="8"/>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" s="11"/>
+      <c r="B49" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="C49" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="D49" s="13" t="s">
+        <v>314</v>
+      </c>
+      <c r="E49" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="F49" s="8"/>
+      <c r="G49" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>